<commit_message>
Did the SQA signoff for conflicts this afternoon
</commit_message>
<xml_diff>
--- a/TestFiles/Test files for conflictTimes/FileIndex.xlsx
+++ b/TestFiles/Test files for conflictTimes/FileIndex.xlsx
@@ -132,9 +132,6 @@
     <t>Input is not accepted. The time is not properly formatted. Missing ":".</t>
   </si>
   <si>
-    <t>Input is not accepted. Line one and line three have duplicate classes.</t>
-  </si>
-  <si>
     <t>Input not accepted. Empty file.</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Input is not accepted. On line one, the days are seperated by a dash. Line two time format is incorrect. A maximum of two digits can follow ":". On line three, only two charcters are allowed after course number and duplicate days/times on the same line.</t>
+  </si>
+  <si>
+    <t>Input is accepted. Line one and line three have duplicate classes so line three will overwrite line one in the database.</t>
   </si>
 </sst>
 </file>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +684,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>26</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>27</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -732,15 +732,15 @@
         <v>30</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>